<commit_message>
i added something to the main code
</commit_message>
<xml_diff>
--- a/2021.xlsx
+++ b/2021.xlsx
@@ -35,9 +35,6 @@
     <t>Year</t>
   </si>
   <si>
-    <t xml:space="preserve">SolRadiation (MJ/m²/day)  </t>
-  </si>
-  <si>
     <t>TempMin (°C)</t>
   </si>
   <si>
@@ -48,6 +45,9 @@
   </si>
   <si>
     <t>RelHumMax (%)</t>
+  </si>
+  <si>
+    <t>SolRadiation</t>
   </si>
 </sst>
 </file>
@@ -443,7 +443,7 @@
   <dimension ref="A1:H366"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,19 +462,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>